<commit_message>
Multiple expiries option chain
</commit_message>
<xml_diff>
--- a/backtest results/Balance.xlsx
+++ b/backtest results/Balance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aniket.bhadane/Desktop/General/AniketBhadane.github.io/backtest results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05D29147-F660-FB41-AF57-101B69AE457C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{075E3F2B-EBC2-4A4E-8819-07F2CD359400}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20140" activeTab="1" xr2:uid="{2F6EBC25-3AA2-2041-A9CD-E7098B4FE5BF}"/>
   </bookViews>
@@ -33693,7 +33693,7 @@
   <dimension ref="B1:AO85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>